<commit_message>
Implement the main(), prog(), opt_stmts(), stmt_lst(), instr() and stmt() functions following the parsing table.
</commit_message>
<xml_diff>
--- a/ParsingTable.xlsx
+++ b/ParsingTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salvador/Desktop/CompilerDesign_Partial2_src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF1A7D5-A53B-BB44-8CA9-4E22AEEFEAAE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53851DCB-CB7B-2341-B8DE-299B635C17D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="8200" windowWidth="28040" windowHeight="17440" xr2:uid="{E79AD578-4051-8245-A8EA-AFE3DB752E6D}"/>
+    <workbookView xWindow="5780" yWindow="9720" windowWidth="28040" windowHeight="17440" xr2:uid="{E79AD578-4051-8245-A8EA-AFE3DB752E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -231,6 +231,9 @@
     <t>stmt -&gt; if (expresion) opt_stmts</t>
   </si>
   <si>
+    <t>stmt -&gt; ifelse (expresion) opt_stmts opt_stmts</t>
+  </si>
+  <si>
     <t>stmt -&gt; while (expresion) opt_stmts</t>
   </si>
   <si>
@@ -274,9 +277,6 @@
   </si>
   <si>
     <t>{*, /, +, -, ;, ), &lt;, &gt;, =}</t>
-  </si>
-  <si>
-    <t>ifelse (expresion) opt_stmts opt_stmts</t>
   </si>
   <si>
     <t xml:space="preserve">opt_stmts -&gt; {stmt_lst} </t>
@@ -543,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -614,6 +614,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -931,7 +934,7 @@
   <dimension ref="A1:V51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="174" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,7 +947,7 @@
     <col min="6" max="6" width="27.83203125" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.83203125" style="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.6640625" style="19" customWidth="1"/>
     <col min="10" max="10" width="31.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.5" style="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.6640625" style="19" bestFit="1" customWidth="1"/>
@@ -1087,25 +1090,25 @@
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
       <c r="I4" s="28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K4" s="29" t="s">
         <v>84</v>
       </c>
       <c r="L4" s="27"/>
       <c r="M4" s="28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N4" s="27"/>
       <c r="O4" s="27"/>
@@ -1133,10 +1136,10 @@
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
       <c r="I5" s="26" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
@@ -1154,7 +1157,7 @@
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26" t="s">
@@ -1183,7 +1186,7 @@
       <c r="U6" s="31"/>
       <c r="V6" s="26"/>
     </row>
-    <row r="7" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="25" t="s">
         <v>4</v>
@@ -1206,7 +1209,7 @@
       </c>
       <c r="K7" s="27"/>
       <c r="L7" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M7" s="32" t="s">
         <v>85</v>
@@ -1229,18 +1232,18 @@
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
       <c r="E8" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
       <c r="I8" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
@@ -1264,12 +1267,12 @@
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="27"/>
       <c r="G9" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H9" s="27"/>
       <c r="I9" s="27"/>
@@ -1282,7 +1285,7 @@
       <c r="P9" s="27"/>
       <c r="Q9" s="27"/>
       <c r="R9" s="27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S9" s="27"/>
       <c r="T9" s="27"/>
@@ -1296,12 +1299,12 @@
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
       <c r="G10" s="26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -1314,7 +1317,7 @@
       <c r="P10" s="26"/>
       <c r="Q10" s="26"/>
       <c r="R10" s="26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S10" s="26"/>
       <c r="T10" s="26"/>
@@ -1368,12 +1371,12 @@
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="26"/>
       <c r="G12" s="26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -1386,7 +1389,7 @@
       <c r="P12" s="26"/>
       <c r="Q12" s="26"/>
       <c r="R12" s="30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="S12" s="26"/>
       <c r="T12" s="26"/>
@@ -1404,20 +1407,20 @@
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
       <c r="L13" s="27"/>
       <c r="M13" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N13" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O13" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P13" s="27" t="s">
         <v>90</v>
@@ -1427,18 +1430,18 @@
       </c>
       <c r="R13" s="27"/>
       <c r="S13" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T13" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="U13" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="V13" s="27"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
       <c r="B14" s="25" t="s">
         <v>93</v>
       </c>
@@ -1469,8 +1472,8 @@
       </c>
       <c r="V14" s="26"/>
     </row>
-    <row r="15" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="36"/>
       <c r="B15" s="33"/>
     </row>
     <row r="16" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1702,7 +1705,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B44" s="23" t="s">
         <v>39</v>
@@ -1716,7 +1719,7 @@
         <v>4</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>51</v>
@@ -1730,7 +1733,7 @@
         <v>40</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D46" s="35"/>
       <c r="E46" s="34"/>
@@ -1744,7 +1747,7 @@
         <v>39</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1766,7 +1769,7 @@
         <v>39</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1777,7 +1780,7 @@
         <v>42</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1793,9 +1796,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A3:A14"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:V1"/>
-    <mergeCell ref="A3:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement the remaining functions. All nine tests are passing.
</commit_message>
<xml_diff>
--- a/ParsingTable.xlsx
+++ b/ParsingTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salvador/Desktop/CompilerDesign_Partial2_src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53851DCB-CB7B-2341-B8DE-299B635C17D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A28A29-9D76-064B-B9BF-18469443A5FA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="9720" windowWidth="28040" windowHeight="17440" xr2:uid="{E79AD578-4051-8245-A8EA-AFE3DB752E6D}"/>
+    <workbookView xWindow="460" yWindow="4900" windowWidth="28040" windowHeight="17440" xr2:uid="{E79AD578-4051-8245-A8EA-AFE3DB752E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197305F2-2BBF-184E-AF8B-40AA57DAFEB0}">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="174" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="174" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>